<commit_message>
small change in BLK
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="1360" windowWidth="28160" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="3260" yWindow="1120" windowWidth="28160" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BLK" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>The number of total instances in the two classes: 11757</t>
   </si>
@@ -53,12 +53,6 @@
     <t>no noise</t>
   </si>
   <si>
-    <t xml:space="preserve">Training time without validation: 0.466959 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test time for all test data: 0.282356 </t>
-  </si>
-  <si>
     <t>The number of total instances in the two classes: 11819</t>
   </si>
   <si>
@@ -134,12 +128,6 @@
     <t>Wire and facade</t>
   </si>
   <si>
-    <t xml:space="preserve">Training time without validation: 0.295501 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test time for all test data: 0.282624 </t>
-  </si>
-  <si>
     <t>The number of total instances in the two classes: 6053</t>
   </si>
   <si>
@@ -174,6 +162,48 @@
   </si>
   <si>
     <t xml:space="preserve"> [ 172 4923]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training time without validation: 0.328284 </t>
+  </si>
+  <si>
+    <t>The number of total instances in the two classes: 13948</t>
+  </si>
+  <si>
+    <t>The number of correctlly classified: 13003</t>
+  </si>
+  <si>
+    <t>The accuracy of classification: 93.22 %</t>
+  </si>
+  <si>
+    <t>[[ 1607   625]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  320 11396]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test time for all test data: 0.302620 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training time without validation: 0.444265 </t>
+  </si>
+  <si>
+    <t>The number of total instances in the two classes: 27432</t>
+  </si>
+  <si>
+    <t>The number of correctlly classified: 25462</t>
+  </si>
+  <si>
+    <t>The accuracy of classification: 92.82 %</t>
+  </si>
+  <si>
+    <t>[[14880   836]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 1134 10582]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test time for all test data: 0.256323 </t>
   </si>
 </sst>
 </file>
@@ -488,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J23"/>
+  <dimension ref="B1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,7 +534,7 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
@@ -515,85 +545,85 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
@@ -607,107 +637,167 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>34</v>
+      <c r="C13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
         <v>35</v>
       </c>
-      <c r="F16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
         <v>36</v>
       </c>
-      <c r="F17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>37</v>
-      </c>
-      <c r="F18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>